<commit_message>
alle navn fra skiforbundet.no
</commit_message>
<xml_diff>
--- a/gutter-jr.xlsx
+++ b/gutter-jr.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28820" windowHeight="20460" tabRatio="991" activeTab="13"/>
+    <workbookView xWindow="19080" yWindow="460" windowWidth="14520" windowHeight="20460" tabRatio="991"/>
   </bookViews>
   <sheets>
     <sheet name="K1" sheetId="1" r:id="rId1"/>
@@ -161,7 +161,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="60">
   <si>
     <t>Dag1</t>
   </si>
@@ -274,61 +274,73 @@
     <t>Tour de Synnfjell Sammenlagt - Gutter 17-20</t>
   </si>
   <si>
-    <t>Rune Hermundstad Grobakken</t>
+    <t>Dragerengen, Ivar</t>
   </si>
   <si>
-    <t>Morten Ramstad</t>
+    <t>Eriksen, Christian Opsahl</t>
   </si>
   <si>
-    <t>Christian Opsahl Eriksen</t>
+    <t>Granvold, Simen</t>
   </si>
   <si>
-    <t>Nils Henrik Kvale</t>
+    <t>Grobakken, Rune Hermundstad</t>
   </si>
   <si>
-    <t>Arngrim Sørumshagen</t>
+    <t>Haugnes, Mathias Bjerregård</t>
   </si>
   <si>
-    <t>Mathias Bjerregård Haugnes</t>
+    <t>Kvale, Nils Henrik</t>
   </si>
   <si>
-    <t>Bendik Lae Steinsrud</t>
+    <t>Lindmoen, Petter</t>
   </si>
   <si>
-    <t>Eirik Seegård</t>
+    <t>Ramstad, Morten</t>
   </si>
   <si>
-    <t>Markus Moen Riste</t>
+    <t>Riste, Markus Moen</t>
   </si>
   <si>
-    <t>Petter Lindmoen</t>
+    <t>Seegard, Eirik</t>
   </si>
   <si>
-    <t>Simen Granvold</t>
+    <t>Steinsrud, Bendik Lae</t>
   </si>
   <si>
-    <t>Ivar Dragerengen</t>
+    <t>Sørumshagen, Arngrim</t>
   </si>
   <si>
-    <t>Kristoffer Seegaard</t>
+    <t>Bossum, Andreas</t>
   </si>
   <si>
-    <t>Vidar Brenna</t>
+    <t>Brenna, Vidar</t>
   </si>
   <si>
-    <t>Marius Viken Vesterås</t>
+    <t>Flugstad, Fredrik Fuglerud</t>
   </si>
   <si>
-    <t>Thomas Stangjordet</t>
+    <t>Moseby, Håvard</t>
   </si>
   <si>
-    <t>Håvard Moseby</t>
+    <t>Seegaard, Kristoffer</t>
   </si>
   <si>
-    <t>Fredrik Fuglerud Flugstad</t>
+    <t>Stangjordet, Thomas</t>
   </si>
   <si>
-    <t>Andreas Bossum</t>
+    <t>Vesterås, Marius Viken</t>
+  </si>
+  <si>
+    <t>Evensen, Ansgar</t>
+  </si>
+  <si>
+    <t>Karsrud, Kristoffer Alm</t>
+  </si>
+  <si>
+    <t>Nyhagen, Håkon</t>
+  </si>
+  <si>
+    <t>Stensvold, Trym</t>
   </si>
 </sst>
 </file>
@@ -931,8 +943,8 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:M104"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="185" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="185" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1551,33 +1563,35 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="13"/>
+      <c r="A16" s="13" t="s">
+        <v>56</v>
+      </c>
       <c r="B16" s="25"/>
       <c r="C16" s="10" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D16" s="11" t="str">
         <f>IF(A16="","", IFERROR(VLOOKUP(C16,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="E16" s="25"/>
       <c r="F16" s="10" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="G16" s="11" t="str">
         <f>IF(A16="","",IFERROR(VLOOKUP(F16,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="H16" s="25"/>
       <c r="I16" s="10" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="J16" s="12" t="str">
         <f>IF(A16="","",IFERROR(VLOOKUP(I16,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="K16" s="26" t="str">
         <f t="shared" si="3"/>
@@ -1585,41 +1599,43 @@
       </c>
       <c r="L16" s="10" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="M16" s="12" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>-</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="13"/>
+      <c r="A17" s="13" t="s">
+        <v>57</v>
+      </c>
       <c r="B17" s="25"/>
       <c r="C17" s="10" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D17" s="11" t="str">
         <f>IF(A17="","", IFERROR(VLOOKUP(C17,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="E17" s="25"/>
       <c r="F17" s="10" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="G17" s="11" t="str">
         <f>IF(A17="","",IFERROR(VLOOKUP(F17,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="H17" s="25"/>
       <c r="I17" s="10" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="J17" s="12" t="str">
         <f>IF(A17="","",IFERROR(VLOOKUP(I17,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="K17" s="26" t="str">
         <f t="shared" si="3"/>
@@ -1627,41 +1643,43 @@
       </c>
       <c r="L17" s="10" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="M17" s="12" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>-</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" s="13"/>
+      <c r="A18" s="13" t="s">
+        <v>58</v>
+      </c>
       <c r="B18" s="25"/>
       <c r="C18" s="10" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D18" s="11" t="str">
         <f>IF(A18="","", IFERROR(VLOOKUP(C18,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="E18" s="25"/>
       <c r="F18" s="10" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="G18" s="11" t="str">
         <f>IF(A18="","",IFERROR(VLOOKUP(F18,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="H18" s="25"/>
       <c r="I18" s="10" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="J18" s="12" t="str">
         <f>IF(A18="","",IFERROR(VLOOKUP(I18,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="K18" s="26" t="str">
         <f t="shared" si="3"/>
@@ -1669,41 +1687,43 @@
       </c>
       <c r="L18" s="10" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="M18" s="12" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>-</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="13"/>
+      <c r="A19" s="13" t="s">
+        <v>59</v>
+      </c>
       <c r="B19" s="25"/>
       <c r="C19" s="10" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D19" s="11" t="str">
         <f>IF(A19="","", IFERROR(VLOOKUP(C19,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="E19" s="25"/>
       <c r="F19" s="10" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="G19" s="11" t="str">
         <f>IF(A19="","",IFERROR(VLOOKUP(F19,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="H19" s="25"/>
       <c r="I19" s="10" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="J19" s="12" t="str">
         <f>IF(A19="","",IFERROR(VLOOKUP(I19,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="K19" s="26" t="str">
         <f t="shared" si="3"/>
@@ -1711,11 +1731,11 @@
       </c>
       <c r="L19" s="10" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="M19" s="12" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>-</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
@@ -12908,7 +12928,7 @@
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="str">
         <f>IF('K2'!A7="", "",'K2'!A7)</f>
-        <v>Thomas Stangjordet</v>
+        <v>Moseby, Håvard</v>
       </c>
       <c r="B6" s="19" t="str">
         <f>IF('K2'!B7="", "",'K2'!B7)</f>
@@ -12978,7 +12998,7 @@
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="str">
         <f>IF('K1'!A4="", "",'K1'!A4)</f>
-        <v>Rune Hermundstad Grobakken</v>
+        <v>Dragerengen, Ivar</v>
       </c>
       <c r="B7" s="19" t="str">
         <f>IF('K1'!B4="", "",'K1'!B4)</f>
@@ -13048,7 +13068,7 @@
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="str">
         <f>IF('K1'!A8="", "",'K1'!A8)</f>
-        <v>Arngrim Sørumshagen</v>
+        <v>Haugnes, Mathias Bjerregård</v>
       </c>
       <c r="B8" s="19" t="str">
         <f>IF('K1'!B8="", "",'K1'!B8)</f>
@@ -13118,7 +13138,7 @@
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="str">
         <f>IF('K1'!A9="", "",'K1'!A9)</f>
-        <v>Mathias Bjerregård Haugnes</v>
+        <v>Kvale, Nils Henrik</v>
       </c>
       <c r="B9" s="19" t="str">
         <f>IF('K1'!B9="", "",'K1'!B9)</f>
@@ -13188,7 +13208,7 @@
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="str">
         <f>IF('K1'!A10="", "",'K1'!A10)</f>
-        <v>Bendik Lae Steinsrud</v>
+        <v>Lindmoen, Petter</v>
       </c>
       <c r="B10" s="19" t="str">
         <f>IF('K1'!B10="", "",'K1'!B10)</f>
@@ -13258,7 +13278,7 @@
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="str">
         <f>IF('K1'!A11="", "",'K1'!A11)</f>
-        <v>Eirik Seegård</v>
+        <v>Ramstad, Morten</v>
       </c>
       <c r="B11" s="19" t="str">
         <f>IF('K1'!B11="", "",'K1'!B11)</f>
@@ -13328,7 +13348,7 @@
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="str">
         <f>IF('K1'!A12="", "",'K1'!A12)</f>
-        <v>Markus Moen Riste</v>
+        <v>Riste, Markus Moen</v>
       </c>
       <c r="B12" s="19" t="str">
         <f>IF('K1'!B12="", "",'K1'!B12)</f>
@@ -13398,7 +13418,7 @@
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="str">
         <f>IF('K1'!A13="", "",'K1'!A13)</f>
-        <v>Petter Lindmoen</v>
+        <v>Seegard, Eirik</v>
       </c>
       <c r="B13" s="19" t="str">
         <f>IF('K1'!B13="", "",'K1'!B13)</f>
@@ -13468,7 +13488,7 @@
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="str">
         <f>IF('K1'!A14="", "",'K1'!A14)</f>
-        <v>Simen Granvold</v>
+        <v>Steinsrud, Bendik Lae</v>
       </c>
       <c r="B14" s="19" t="str">
         <f>IF('K1'!B14="", "",'K1'!B14)</f>
@@ -13538,7 +13558,7 @@
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="str">
         <f>IF('K1'!A15="", "",'K1'!A15)</f>
-        <v>Ivar Dragerengen</v>
+        <v>Sørumshagen, Arngrim</v>
       </c>
       <c r="B15" s="19" t="str">
         <f>IF('K1'!B15="", "",'K1'!B15)</f>
@@ -13608,7 +13628,7 @@
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="str">
         <f>IF('K1'!A16="", "",'K1'!A16)</f>
-        <v/>
+        <v>Evensen, Ansgar</v>
       </c>
       <c r="B16" s="19" t="str">
         <f>IF('K1'!B16="", "",'K1'!B16)</f>
@@ -13620,11 +13640,11 @@
       </c>
       <c r="D16" s="23" t="str">
         <f>IF(A16="","",IFERROR(VLOOKUP(E16,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="E16" s="23" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="F16" s="19" t="str">
         <f>IF('K1'!E16="", "", 'K1'!E16)</f>
@@ -13636,11 +13656,11 @@
       </c>
       <c r="H16" s="23" t="str">
         <f>IF(A16="","",IFERROR(VLOOKUP(I16,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="I16" s="23" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="J16" s="19" t="str">
         <f>IF('K1'!H16="", "", 'K1'!H16)</f>
@@ -13652,11 +13672,11 @@
       </c>
       <c r="L16" s="23" t="str">
         <f>IF(A16="","",IFERROR(VLOOKUP(M16,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="M16" s="23" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="N16" s="27" t="str">
         <f>IF('K1'!K16="", "", 'K1'!K16)</f>
@@ -13668,17 +13688,17 @@
       </c>
       <c r="P16" s="23" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="Q16" s="23" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>-</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="str">
         <f>IF('K1'!A17="", "",'K1'!A17)</f>
-        <v/>
+        <v>Karsrud, Kristoffer Alm</v>
       </c>
       <c r="B17" s="19" t="str">
         <f>IF('K1'!B17="", "",'K1'!B17)</f>
@@ -13690,11 +13710,11 @@
       </c>
       <c r="D17" s="23" t="str">
         <f>IF(A17="","",IFERROR(VLOOKUP(E17,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="E17" s="23" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="F17" s="19" t="str">
         <f>IF('K1'!E17="", "", 'K1'!E17)</f>
@@ -13706,11 +13726,11 @@
       </c>
       <c r="H17" s="23" t="str">
         <f>IF(A17="","",IFERROR(VLOOKUP(I17,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="I17" s="23" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="J17" s="19" t="str">
         <f>IF('K1'!H17="", "", 'K1'!H17)</f>
@@ -13722,11 +13742,11 @@
       </c>
       <c r="L17" s="23" t="str">
         <f>IF(A17="","",IFERROR(VLOOKUP(M17,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="M17" s="23" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="N17" s="27" t="str">
         <f>IF('K1'!K17="", "", 'K1'!K17)</f>
@@ -13738,17 +13758,17 @@
       </c>
       <c r="P17" s="23" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="Q17" s="23" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>-</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="str">
         <f>IF('K1'!A18="", "",'K1'!A18)</f>
-        <v/>
+        <v>Nyhagen, Håkon</v>
       </c>
       <c r="B18" s="19" t="str">
         <f>IF('K1'!B18="", "",'K1'!B18)</f>
@@ -13760,11 +13780,11 @@
       </c>
       <c r="D18" s="23" t="str">
         <f>IF(A18="","",IFERROR(VLOOKUP(E18,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="E18" s="23" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="F18" s="19" t="str">
         <f>IF('K1'!E18="", "", 'K1'!E18)</f>
@@ -13776,11 +13796,11 @@
       </c>
       <c r="H18" s="23" t="str">
         <f>IF(A18="","",IFERROR(VLOOKUP(I18,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="I18" s="23" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="J18" s="19" t="str">
         <f>IF('K1'!H18="", "", 'K1'!H18)</f>
@@ -13792,11 +13812,11 @@
       </c>
       <c r="L18" s="23" t="str">
         <f>IF(A18="","",IFERROR(VLOOKUP(M18,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="M18" s="23" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="N18" s="27" t="str">
         <f>IF('K1'!K18="", "", 'K1'!K18)</f>
@@ -13808,17 +13828,17 @@
       </c>
       <c r="P18" s="23" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="Q18" s="23" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>-</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="str">
         <f>IF('K1'!A19="", "",'K1'!A19)</f>
-        <v/>
+        <v>Stensvold, Trym</v>
       </c>
       <c r="B19" s="19" t="str">
         <f>IF('K1'!B19="", "",'K1'!B19)</f>
@@ -13830,11 +13850,11 @@
       </c>
       <c r="D19" s="23" t="str">
         <f>IF(A19="","",IFERROR(VLOOKUP(E19,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="E19" s="23" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="F19" s="19" t="str">
         <f>IF('K1'!E19="", "", 'K1'!E19)</f>
@@ -13846,11 +13866,11 @@
       </c>
       <c r="H19" s="23" t="str">
         <f>IF(A19="","",IFERROR(VLOOKUP(I19,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="I19" s="23" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="J19" s="19" t="str">
         <f>IF('K1'!H19="", "", 'K1'!H19)</f>
@@ -13862,11 +13882,11 @@
       </c>
       <c r="L19" s="23" t="str">
         <f>IF(A19="","",IFERROR(VLOOKUP(M19,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="M19" s="23" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="N19" s="27" t="str">
         <f>IF('K1'!K19="", "", 'K1'!K19)</f>
@@ -13878,11 +13898,11 @@
       </c>
       <c r="P19" s="23" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="Q19" s="23" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>-</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
@@ -19838,7 +19858,7 @@
     <row r="105" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A105" s="15" t="str">
         <f>IF('K2'!A4="", "",'K2'!A4)</f>
-        <v>Kristoffer Seegaard</v>
+        <v>Bossum, Andreas</v>
       </c>
       <c r="B105" s="19" t="str">
         <f>IF('K2'!B4="", "",'K2'!B4)</f>
@@ -19908,7 +19928,7 @@
     <row r="106" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A106" s="15" t="str">
         <f>IF('K1'!A5="", "",'K1'!A5)</f>
-        <v>Morten Ramstad</v>
+        <v>Eriksen, Christian Opsahl</v>
       </c>
       <c r="B106" s="19" t="str">
         <f>IF('K1'!B5="", "",'K1'!B5)</f>
@@ -19978,7 +19998,7 @@
     <row r="107" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A107" s="15" t="str">
         <f>IF('K2'!A6="", "",'K2'!A6)</f>
-        <v>Marius Viken Vesterås</v>
+        <v>Flugstad, Fredrik Fuglerud</v>
       </c>
       <c r="B107" s="19" t="str">
         <f>IF('K2'!B6="", "",'K2'!B6)</f>
@@ -20048,7 +20068,7 @@
     <row r="108" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A108" s="15" t="str">
         <f>IF('K2'!A8="", "",'K2'!A8)</f>
-        <v>Håvard Moseby</v>
+        <v>Seegaard, Kristoffer</v>
       </c>
       <c r="B108" s="19" t="str">
         <f>IF('K2'!B8="", "",'K2'!B8)</f>
@@ -20118,7 +20138,7 @@
     <row r="109" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A109" s="15" t="str">
         <f>IF('K2'!A9="", "",'K2'!A9)</f>
-        <v>Fredrik Fuglerud Flugstad</v>
+        <v>Stangjordet, Thomas</v>
       </c>
       <c r="B109" s="19" t="str">
         <f>IF('K2'!B9="", "",'K2'!B9)</f>
@@ -20188,7 +20208,7 @@
     <row r="110" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A110" s="15" t="str">
         <f>IF('K2'!A10="", "",'K2'!A10)</f>
-        <v>Andreas Bossum</v>
+        <v>Vesterås, Marius Viken</v>
       </c>
       <c r="B110" s="19" t="str">
         <f>IF('K2'!B10="", "",'K2'!B10)</f>
@@ -26768,7 +26788,7 @@
     <row r="204" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A204" s="15" t="str">
         <f>IF('K2'!A5="", "",'K2'!A5)</f>
-        <v>Vidar Brenna</v>
+        <v>Brenna, Vidar</v>
       </c>
       <c r="B204" s="19" t="str">
         <f>IF('K2'!B5="", "",'K2'!B5)</f>
@@ -26838,7 +26858,7 @@
     <row r="205" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A205" s="15" t="str">
         <f>IF('K1'!A7="", "",'K1'!A7)</f>
-        <v>Nils Henrik Kvale</v>
+        <v>Grobakken, Rune Hermundstad</v>
       </c>
       <c r="B205" s="19" t="str">
         <f>IF('K1'!B7="", "",'K1'!B7)</f>
@@ -26908,7 +26928,7 @@
     <row r="206" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A206" s="15" t="str">
         <f>IF('K1'!A6="", "",'K1'!A6)</f>
-        <v>Christian Opsahl Eriksen</v>
+        <v>Granvold, Simen</v>
       </c>
       <c r="B206" s="19" t="str">
         <f>IF('K1'!B6="", "",'K1'!B6)</f>
@@ -33794,7 +33814,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M303"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="185" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="185" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -33910,7 +33930,7 @@
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="39" t="str">
         <f>IF(D1D2D3!A7="", "",D1D2D3!A7)</f>
-        <v>Rune Hermundstad Grobakken</v>
+        <v>Dragerengen, Ivar</v>
       </c>
       <c r="B6" s="41" t="str">
         <f>IF(D1D2D3!A7="", "",D1D2D3!P7)</f>
@@ -33934,7 +33954,7 @@
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="39" t="str">
         <f>IF(D1D2D3!A6="", "",D1D2D3!A6)</f>
-        <v>Thomas Stangjordet</v>
+        <v>Moseby, Håvard</v>
       </c>
       <c r="B7" s="41" t="str">
         <f>IF(D1D2D3!A6="", "",D1D2D3!P6)</f>
@@ -33958,7 +33978,7 @@
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="39" t="str">
         <f>IF(D1D2D3!A8="", "",D1D2D3!A8)</f>
-        <v>Arngrim Sørumshagen</v>
+        <v>Haugnes, Mathias Bjerregård</v>
       </c>
       <c r="B8" s="41" t="str">
         <f>IF(D1D2D3!A8="", "",D1D2D3!P8)</f>
@@ -33982,7 +34002,7 @@
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="39" t="str">
         <f>IF(D1D2D3!A9="", "",D1D2D3!A9)</f>
-        <v>Mathias Bjerregård Haugnes</v>
+        <v>Kvale, Nils Henrik</v>
       </c>
       <c r="B9" s="41" t="str">
         <f>IF(D1D2D3!A9="", "",D1D2D3!P9)</f>
@@ -34006,7 +34026,7 @@
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="39" t="str">
         <f>IF(D1D2D3!A10="", "",D1D2D3!A10)</f>
-        <v>Bendik Lae Steinsrud</v>
+        <v>Lindmoen, Petter</v>
       </c>
       <c r="B10" s="41" t="str">
         <f>IF(D1D2D3!A10="", "",D1D2D3!P10)</f>
@@ -34030,7 +34050,7 @@
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="39" t="str">
         <f>IF(D1D2D3!A11="", "",D1D2D3!A11)</f>
-        <v>Eirik Seegård</v>
+        <v>Ramstad, Morten</v>
       </c>
       <c r="B11" s="41" t="str">
         <f>IF(D1D2D3!A11="", "",D1D2D3!P11)</f>
@@ -34054,7 +34074,7 @@
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="39" t="str">
         <f>IF(D1D2D3!A12="", "",D1D2D3!A12)</f>
-        <v>Markus Moen Riste</v>
+        <v>Riste, Markus Moen</v>
       </c>
       <c r="B12" s="41" t="str">
         <f>IF(D1D2D3!A12="", "",D1D2D3!P12)</f>
@@ -34078,7 +34098,7 @@
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="39" t="str">
         <f>IF(D1D2D3!A13="", "",D1D2D3!A13)</f>
-        <v>Petter Lindmoen</v>
+        <v>Seegard, Eirik</v>
       </c>
       <c r="B13" s="41" t="str">
         <f>IF(D1D2D3!A13="", "",D1D2D3!P13)</f>
@@ -34102,7 +34122,7 @@
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="39" t="str">
         <f>IF(D1D2D3!A14="", "",D1D2D3!A14)</f>
-        <v>Simen Granvold</v>
+        <v>Steinsrud, Bendik Lae</v>
       </c>
       <c r="B14" s="41" t="str">
         <f>IF(D1D2D3!A14="", "",D1D2D3!P14)</f>
@@ -34126,7 +34146,7 @@
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="39" t="str">
         <f>IF(D1D2D3!A15="", "",D1D2D3!A15)</f>
-        <v>Ivar Dragerengen</v>
+        <v>Sørumshagen, Arngrim</v>
       </c>
       <c r="B15" s="41" t="str">
         <f>IF(D1D2D3!A15="", "",D1D2D3!P15)</f>
@@ -34150,15 +34170,15 @@
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="39" t="str">
         <f>IF(D1D2D3!A16="", "",D1D2D3!A16)</f>
-        <v/>
+        <v>Evensen, Ansgar</v>
       </c>
       <c r="B16" s="41" t="str">
         <f>IF(D1D2D3!A16="", "",D1D2D3!P16)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="C16" s="37" t="str">
         <f>IF(D1D2D3!A16="", "",D1D2D3!Q16)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D16" s="11"/>
       <c r="E16" s="25"/>
@@ -34174,15 +34194,15 @@
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="39" t="str">
         <f>IF(D1D2D3!A17="", "",D1D2D3!A17)</f>
-        <v/>
+        <v>Karsrud, Kristoffer Alm</v>
       </c>
       <c r="B17" s="41" t="str">
         <f>IF(D1D2D3!A17="", "",D1D2D3!P17)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="C17" s="37" t="str">
         <f>IF(D1D2D3!A17="", "",D1D2D3!Q17)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D17" s="11"/>
       <c r="E17" s="25"/>
@@ -34198,15 +34218,15 @@
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="39" t="str">
         <f>IF(D1D2D3!A18="", "",D1D2D3!A18)</f>
-        <v/>
+        <v>Nyhagen, Håkon</v>
       </c>
       <c r="B18" s="41" t="str">
         <f>IF(D1D2D3!A18="", "",D1D2D3!P18)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="C18" s="37" t="str">
         <f>IF(D1D2D3!A18="", "",D1D2D3!Q18)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D18" s="11"/>
       <c r="E18" s="25"/>
@@ -34222,15 +34242,15 @@
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="39" t="str">
         <f>IF(D1D2D3!A19="", "",D1D2D3!A19)</f>
-        <v/>
+        <v>Stensvold, Trym</v>
       </c>
       <c r="B19" s="41" t="str">
         <f>IF(D1D2D3!A19="", "",D1D2D3!P19)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="C19" s="37" t="str">
         <f>IF(D1D2D3!A19="", "",D1D2D3!Q19)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D19" s="11"/>
       <c r="E19" s="25"/>
@@ -36257,7 +36277,7 @@
     <row r="105" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A105" s="39" t="str">
         <f>IF(D1D2D3!A105="", "",D1D2D3!A105)</f>
-        <v>Kristoffer Seegaard</v>
+        <v>Bossum, Andreas</v>
       </c>
       <c r="B105" s="41" t="str">
         <f>IF(D1D2D3!A105="", "",D1D2D3!P105)</f>
@@ -36271,7 +36291,7 @@
     <row r="106" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A106" s="39" t="str">
         <f>IF(D1D2D3!A106="", "",D1D2D3!A106)</f>
-        <v>Morten Ramstad</v>
+        <v>Eriksen, Christian Opsahl</v>
       </c>
       <c r="B106" s="41" t="str">
         <f>IF(D1D2D3!A106="", "",D1D2D3!P106)</f>
@@ -36285,7 +36305,7 @@
     <row r="107" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A107" s="39" t="str">
         <f>IF(D1D2D3!A107="", "",D1D2D3!A107)</f>
-        <v>Marius Viken Vesterås</v>
+        <v>Flugstad, Fredrik Fuglerud</v>
       </c>
       <c r="B107" s="41" t="str">
         <f>IF(D1D2D3!A107="", "",D1D2D3!P107)</f>
@@ -36299,7 +36319,7 @@
     <row r="108" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A108" s="39" t="str">
         <f>IF(D1D2D3!A108="", "",D1D2D3!A108)</f>
-        <v>Håvard Moseby</v>
+        <v>Seegaard, Kristoffer</v>
       </c>
       <c r="B108" s="41" t="str">
         <f>IF(D1D2D3!A108="", "",D1D2D3!P108)</f>
@@ -36313,7 +36333,7 @@
     <row r="109" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A109" s="39" t="str">
         <f>IF(D1D2D3!A109="", "",D1D2D3!A109)</f>
-        <v>Fredrik Fuglerud Flugstad</v>
+        <v>Stangjordet, Thomas</v>
       </c>
       <c r="B109" s="41" t="str">
         <f>IF(D1D2D3!A109="", "",D1D2D3!P109)</f>
@@ -36327,7 +36347,7 @@
     <row r="110" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A110" s="39" t="str">
         <f>IF(D1D2D3!A110="", "",D1D2D3!A110)</f>
-        <v>Andreas Bossum</v>
+        <v>Vesterås, Marius Viken</v>
       </c>
       <c r="B110" s="41" t="str">
         <f>IF(D1D2D3!A110="", "",D1D2D3!P110)</f>
@@ -37643,7 +37663,7 @@
     <row r="204" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A204" s="39" t="str">
         <f>IF(D1D2D3!A205="", "",D1D2D3!A205)</f>
-        <v>Nils Henrik Kvale</v>
+        <v>Grobakken, Rune Hermundstad</v>
       </c>
       <c r="B204" s="41" t="str">
         <f>IF(D1D2D3!A205="", "",D1D2D3!P205)</f>
@@ -37657,7 +37677,7 @@
     <row r="205" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A205" s="39" t="str">
         <f>IF(D1D2D3!A206="", "",D1D2D3!A206)</f>
-        <v>Christian Opsahl Eriksen</v>
+        <v>Granvold, Simen</v>
       </c>
       <c r="B205" s="41" t="str">
         <f>IF(D1D2D3!A206="", "",D1D2D3!P206)</f>
@@ -39029,7 +39049,7 @@
     <row r="303" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A303" s="39" t="str">
         <f>IF(D1D2D3!A204="", "",D1D2D3!A204)</f>
-        <v>Vidar Brenna</v>
+        <v>Brenna, Vidar</v>
       </c>
       <c r="B303" s="41" t="str">
         <f>IF(D1D2D3!A204="", "",D1D2D3!P204)</f>
@@ -39834,7 +39854,7 @@
   <dimension ref="A1:M104"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="185" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -48541,7 +48561,7 @@
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="39" t="str">
         <f>IF('K1'!A4="", "",'K1'!A4)</f>
-        <v>Rune Hermundstad Grobakken</v>
+        <v>Dragerengen, Ivar</v>
       </c>
       <c r="B4" s="36">
         <f>IF('K1'!A4="", "",'K1'!B4)</f>
@@ -48565,7 +48585,7 @@
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="39" t="str">
         <f>IF('K1'!A5="", "",'K1'!A5)</f>
-        <v>Morten Ramstad</v>
+        <v>Eriksen, Christian Opsahl</v>
       </c>
       <c r="B5" s="36">
         <f>IF('K1'!A5="", "",'K1'!B5)</f>
@@ -48589,7 +48609,7 @@
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="39" t="str">
         <f>IF('K1'!A6="", "",'K1'!A6)</f>
-        <v>Christian Opsahl Eriksen</v>
+        <v>Granvold, Simen</v>
       </c>
       <c r="B6" s="36">
         <f>IF('K1'!A6="", "",'K1'!B6)</f>
@@ -48613,7 +48633,7 @@
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="39" t="str">
         <f>IF('K1'!A7="", "",'K1'!A7)</f>
-        <v>Nils Henrik Kvale</v>
+        <v>Grobakken, Rune Hermundstad</v>
       </c>
       <c r="B7" s="36">
         <f>IF('K1'!A7="", "",'K1'!B7)</f>
@@ -48637,7 +48657,7 @@
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="39" t="str">
         <f>IF('K1'!A8="", "",'K1'!A8)</f>
-        <v>Arngrim Sørumshagen</v>
+        <v>Haugnes, Mathias Bjerregård</v>
       </c>
       <c r="B8" s="36">
         <f>IF('K1'!A8="", "",'K1'!B8)</f>
@@ -48661,7 +48681,7 @@
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="39" t="str">
         <f>IF('K1'!A9="", "",'K1'!A9)</f>
-        <v>Mathias Bjerregård Haugnes</v>
+        <v>Kvale, Nils Henrik</v>
       </c>
       <c r="B9" s="36">
         <f>IF('K1'!A9="", "",'K1'!B9)</f>
@@ -48685,7 +48705,7 @@
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="39" t="str">
         <f>IF('K1'!A10="", "",'K1'!A10)</f>
-        <v>Bendik Lae Steinsrud</v>
+        <v>Lindmoen, Petter</v>
       </c>
       <c r="B10" s="36">
         <f>IF('K1'!A10="", "",'K1'!B10)</f>
@@ -48709,7 +48729,7 @@
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="39" t="str">
         <f>IF('K1'!A11="", "",'K1'!A11)</f>
-        <v>Eirik Seegård</v>
+        <v>Ramstad, Morten</v>
       </c>
       <c r="B11" s="36">
         <f>IF('K1'!A11="", "",'K1'!B11)</f>
@@ -48733,7 +48753,7 @@
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="39" t="str">
         <f>IF('K1'!A12="", "",'K1'!A12)</f>
-        <v>Markus Moen Riste</v>
+        <v>Riste, Markus Moen</v>
       </c>
       <c r="B12" s="36">
         <f>IF('K1'!A12="", "",'K1'!B12)</f>
@@ -48757,7 +48777,7 @@
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="39" t="str">
         <f>IF('K1'!A13="", "",'K1'!A13)</f>
-        <v>Petter Lindmoen</v>
+        <v>Seegard, Eirik</v>
       </c>
       <c r="B13" s="36">
         <f>IF('K1'!A13="", "",'K1'!B13)</f>
@@ -48781,7 +48801,7 @@
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="39" t="str">
         <f>IF('K1'!A14="", "",'K1'!A14)</f>
-        <v>Simen Granvold</v>
+        <v>Steinsrud, Bendik Lae</v>
       </c>
       <c r="B14" s="36">
         <f>IF('K1'!A14="", "",'K1'!B14)</f>
@@ -48805,7 +48825,7 @@
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="39" t="str">
         <f>IF('K1'!A15="", "",'K1'!A15)</f>
-        <v>Ivar Dragerengen</v>
+        <v>Sørumshagen, Arngrim</v>
       </c>
       <c r="B15" s="36">
         <f>IF('K1'!A15="", "",'K1'!B15)</f>
@@ -48829,15 +48849,15 @@
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="39" t="str">
         <f>IF('K1'!A16="", "",'K1'!A16)</f>
-        <v/>
-      </c>
-      <c r="B16" s="36" t="str">
+        <v>Evensen, Ansgar</v>
+      </c>
+      <c r="B16" s="36">
         <f>IF('K1'!A16="", "",'K1'!B16)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C16" s="37" t="str">
         <f>IF('K1'!A16="", "",'K1'!C16)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D16" s="35"/>
       <c r="E16" s="36"/>
@@ -48853,15 +48873,15 @@
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="39" t="str">
         <f>IF('K1'!A17="", "",'K1'!A17)</f>
-        <v/>
-      </c>
-      <c r="B17" s="36" t="str">
+        <v>Karsrud, Kristoffer Alm</v>
+      </c>
+      <c r="B17" s="36">
         <f>IF('K1'!A17="", "",'K1'!B17)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C17" s="37" t="str">
         <f>IF('K1'!A17="", "",'K1'!C17)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D17" s="35"/>
       <c r="E17" s="36"/>
@@ -48877,15 +48897,15 @@
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="39" t="str">
         <f>IF('K1'!A18="", "",'K1'!A18)</f>
-        <v/>
-      </c>
-      <c r="B18" s="36" t="str">
+        <v>Nyhagen, Håkon</v>
+      </c>
+      <c r="B18" s="36">
         <f>IF('K1'!A18="", "",'K1'!B18)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C18" s="37" t="str">
         <f>IF('K1'!A18="", "",'K1'!C18)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D18" s="35"/>
       <c r="E18" s="36"/>
@@ -48901,15 +48921,15 @@
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="39" t="str">
         <f>IF('K1'!A19="", "",'K1'!A19)</f>
-        <v/>
-      </c>
-      <c r="B19" s="36" t="str">
+        <v>Stensvold, Trym</v>
+      </c>
+      <c r="B19" s="36">
         <f>IF('K1'!A19="", "",'K1'!B19)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C19" s="37" t="str">
         <f>IF('K1'!A19="", "",'K1'!C19)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D19" s="35"/>
       <c r="E19" s="36"/>
@@ -51000,7 +51020,7 @@
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="str">
         <f>IF('K1'!A4="", "",'K1'!A4)</f>
-        <v>Rune Hermundstad Grobakken</v>
+        <v>Dragerengen, Ivar</v>
       </c>
       <c r="B4" s="25">
         <f>IF('K1'!A4="", "",'K1'!E4)</f>
@@ -51024,7 +51044,7 @@
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="str">
         <f>IF('K1'!A5="", "",'K1'!A5)</f>
-        <v>Morten Ramstad</v>
+        <v>Eriksen, Christian Opsahl</v>
       </c>
       <c r="B5" s="25">
         <f>IF('K1'!A5="", "",'K1'!E5)</f>
@@ -51048,7 +51068,7 @@
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="str">
         <f>IF('K1'!A6="", "",'K1'!A6)</f>
-        <v>Christian Opsahl Eriksen</v>
+        <v>Granvold, Simen</v>
       </c>
       <c r="B6" s="25">
         <f>IF('K1'!A6="", "",'K1'!E6)</f>
@@ -51072,7 +51092,7 @@
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="str">
         <f>IF('K1'!A7="", "",'K1'!A7)</f>
-        <v>Nils Henrik Kvale</v>
+        <v>Grobakken, Rune Hermundstad</v>
       </c>
       <c r="B7" s="25">
         <f>IF('K1'!A7="", "",'K1'!E7)</f>
@@ -51096,7 +51116,7 @@
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="str">
         <f>IF('K1'!A8="", "",'K1'!A8)</f>
-        <v>Arngrim Sørumshagen</v>
+        <v>Haugnes, Mathias Bjerregård</v>
       </c>
       <c r="B8" s="25">
         <f>IF('K1'!A8="", "",'K1'!E8)</f>
@@ -51120,7 +51140,7 @@
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="str">
         <f>IF('K1'!A9="", "",'K1'!A9)</f>
-        <v>Mathias Bjerregård Haugnes</v>
+        <v>Kvale, Nils Henrik</v>
       </c>
       <c r="B9" s="25">
         <f>IF('K1'!A9="", "",'K1'!E9)</f>
@@ -51144,7 +51164,7 @@
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="str">
         <f>IF('K1'!A10="", "",'K1'!A10)</f>
-        <v>Bendik Lae Steinsrud</v>
+        <v>Lindmoen, Petter</v>
       </c>
       <c r="B10" s="25">
         <f>IF('K1'!A10="", "",'K1'!E10)</f>
@@ -51168,7 +51188,7 @@
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="str">
         <f>IF('K1'!A11="", "",'K1'!A11)</f>
-        <v>Eirik Seegård</v>
+        <v>Ramstad, Morten</v>
       </c>
       <c r="B11" s="25">
         <f>IF('K1'!A11="", "",'K1'!E11)</f>
@@ -51192,7 +51212,7 @@
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="str">
         <f>IF('K1'!A12="", "",'K1'!A12)</f>
-        <v>Markus Moen Riste</v>
+        <v>Riste, Markus Moen</v>
       </c>
       <c r="B12" s="25">
         <f>IF('K1'!A12="", "",'K1'!E12)</f>
@@ -51216,7 +51236,7 @@
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="str">
         <f>IF('K1'!A13="", "",'K1'!A13)</f>
-        <v>Petter Lindmoen</v>
+        <v>Seegard, Eirik</v>
       </c>
       <c r="B13" s="25">
         <f>IF('K1'!A13="", "",'K1'!E13)</f>
@@ -51240,7 +51260,7 @@
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="str">
         <f>IF('K1'!A14="", "",'K1'!A14)</f>
-        <v>Simen Granvold</v>
+        <v>Steinsrud, Bendik Lae</v>
       </c>
       <c r="B14" s="25">
         <f>IF('K1'!A14="", "",'K1'!E14)</f>
@@ -51264,7 +51284,7 @@
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="str">
         <f>IF('K1'!A15="", "",'K1'!A15)</f>
-        <v>Ivar Dragerengen</v>
+        <v>Sørumshagen, Arngrim</v>
       </c>
       <c r="B15" s="25">
         <f>IF('K1'!A15="", "",'K1'!E15)</f>
@@ -51288,15 +51308,15 @@
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="str">
         <f>IF('K1'!A16="", "",'K1'!A16)</f>
-        <v/>
-      </c>
-      <c r="B16" s="25" t="str">
+        <v>Evensen, Ansgar</v>
+      </c>
+      <c r="B16" s="25">
         <f>IF('K1'!A16="", "",'K1'!E16)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C16" s="37" t="str">
         <f>IF('K1'!A16="", "",'K1'!F16)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D16" s="35"/>
       <c r="E16" s="25"/>
@@ -51312,15 +51332,15 @@
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="str">
         <f>IF('K1'!A17="", "",'K1'!A17)</f>
-        <v/>
-      </c>
-      <c r="B17" s="25" t="str">
+        <v>Karsrud, Kristoffer Alm</v>
+      </c>
+      <c r="B17" s="25">
         <f>IF('K1'!A17="", "",'K1'!E17)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C17" s="37" t="str">
         <f>IF('K1'!A17="", "",'K1'!F17)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D17" s="35"/>
       <c r="E17" s="25"/>
@@ -51336,15 +51356,15 @@
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="str">
         <f>IF('K1'!A18="", "",'K1'!A18)</f>
-        <v/>
-      </c>
-      <c r="B18" s="25" t="str">
+        <v>Nyhagen, Håkon</v>
+      </c>
+      <c r="B18" s="25">
         <f>IF('K1'!A18="", "",'K1'!E18)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C18" s="37" t="str">
         <f>IF('K1'!A18="", "",'K1'!F18)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D18" s="35"/>
       <c r="E18" s="25"/>
@@ -51360,15 +51380,15 @@
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="str">
         <f>IF('K1'!A19="", "",'K1'!A19)</f>
-        <v/>
-      </c>
-      <c r="B19" s="25" t="str">
+        <v>Stensvold, Trym</v>
+      </c>
+      <c r="B19" s="25">
         <f>IF('K1'!A19="", "",'K1'!E19)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C19" s="37" t="str">
         <f>IF('K1'!A19="", "",'K1'!F19)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D19" s="35"/>
       <c r="E19" s="25"/>
@@ -53461,7 +53481,7 @@
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="39" t="str">
         <f>IF('K1'!A4="", "",'K1'!A4)</f>
-        <v>Rune Hermundstad Grobakken</v>
+        <v>Dragerengen, Ivar</v>
       </c>
       <c r="B4" s="36">
         <f>IF('K1'!A4="", "",'K1'!H4)</f>
@@ -53485,7 +53505,7 @@
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="39" t="str">
         <f>IF('K1'!A5="", "",'K1'!A5)</f>
-        <v>Morten Ramstad</v>
+        <v>Eriksen, Christian Opsahl</v>
       </c>
       <c r="B5" s="36">
         <f>IF('K1'!A5="", "",'K1'!H5)</f>
@@ -53509,7 +53529,7 @@
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="39" t="str">
         <f>IF('K1'!A6="", "",'K1'!A6)</f>
-        <v>Christian Opsahl Eriksen</v>
+        <v>Granvold, Simen</v>
       </c>
       <c r="B6" s="36">
         <f>IF('K1'!A6="", "",'K1'!H6)</f>
@@ -53533,7 +53553,7 @@
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="39" t="str">
         <f>IF('K1'!A7="", "",'K1'!A7)</f>
-        <v>Nils Henrik Kvale</v>
+        <v>Grobakken, Rune Hermundstad</v>
       </c>
       <c r="B7" s="36">
         <f>IF('K1'!A7="", "",'K1'!H7)</f>
@@ -53557,7 +53577,7 @@
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="39" t="str">
         <f>IF('K1'!A8="", "",'K1'!A8)</f>
-        <v>Arngrim Sørumshagen</v>
+        <v>Haugnes, Mathias Bjerregård</v>
       </c>
       <c r="B8" s="36">
         <f>IF('K1'!A8="", "",'K1'!H8)</f>
@@ -53581,7 +53601,7 @@
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="39" t="str">
         <f>IF('K1'!A9="", "",'K1'!A9)</f>
-        <v>Mathias Bjerregård Haugnes</v>
+        <v>Kvale, Nils Henrik</v>
       </c>
       <c r="B9" s="36">
         <f>IF('K1'!A9="", "",'K1'!H9)</f>
@@ -53605,7 +53625,7 @@
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="39" t="str">
         <f>IF('K1'!A10="", "",'K1'!A10)</f>
-        <v>Bendik Lae Steinsrud</v>
+        <v>Lindmoen, Petter</v>
       </c>
       <c r="B10" s="36">
         <f>IF('K1'!A10="", "",'K1'!H10)</f>
@@ -53629,7 +53649,7 @@
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="39" t="str">
         <f>IF('K1'!A11="", "",'K1'!A11)</f>
-        <v>Eirik Seegård</v>
+        <v>Ramstad, Morten</v>
       </c>
       <c r="B11" s="36">
         <f>IF('K1'!A11="", "",'K1'!H11)</f>
@@ -53653,7 +53673,7 @@
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="39" t="str">
         <f>IF('K1'!A12="", "",'K1'!A12)</f>
-        <v>Markus Moen Riste</v>
+        <v>Riste, Markus Moen</v>
       </c>
       <c r="B12" s="36">
         <f>IF('K1'!A12="", "",'K1'!H12)</f>
@@ -53677,7 +53697,7 @@
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="39" t="str">
         <f>IF('K1'!A13="", "",'K1'!A13)</f>
-        <v>Petter Lindmoen</v>
+        <v>Seegard, Eirik</v>
       </c>
       <c r="B13" s="36">
         <f>IF('K1'!A13="", "",'K1'!H13)</f>
@@ -53701,7 +53721,7 @@
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="39" t="str">
         <f>IF('K1'!A14="", "",'K1'!A14)</f>
-        <v>Simen Granvold</v>
+        <v>Steinsrud, Bendik Lae</v>
       </c>
       <c r="B14" s="36">
         <f>IF('K1'!A14="", "",'K1'!H14)</f>
@@ -53725,7 +53745,7 @@
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="39" t="str">
         <f>IF('K1'!A15="", "",'K1'!A15)</f>
-        <v>Ivar Dragerengen</v>
+        <v>Sørumshagen, Arngrim</v>
       </c>
       <c r="B15" s="36">
         <f>IF('K1'!A15="", "",'K1'!H15)</f>
@@ -53749,15 +53769,15 @@
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="39" t="str">
         <f>IF('K1'!A16="", "",'K1'!A16)</f>
-        <v/>
-      </c>
-      <c r="B16" s="36" t="str">
+        <v>Evensen, Ansgar</v>
+      </c>
+      <c r="B16" s="36">
         <f>IF('K1'!A16="", "",'K1'!H16)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C16" s="37" t="str">
         <f>IF('K1'!A16="", "",'K1'!I16)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D16" s="11"/>
       <c r="E16" s="25"/>
@@ -53773,15 +53793,15 @@
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="39" t="str">
         <f>IF('K1'!A17="", "",'K1'!A17)</f>
-        <v/>
-      </c>
-      <c r="B17" s="36" t="str">
+        <v>Karsrud, Kristoffer Alm</v>
+      </c>
+      <c r="B17" s="36">
         <f>IF('K1'!A17="", "",'K1'!H17)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C17" s="37" t="str">
         <f>IF('K1'!A17="", "",'K1'!I17)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D17" s="11"/>
       <c r="E17" s="25"/>
@@ -53797,15 +53817,15 @@
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="39" t="str">
         <f>IF('K1'!A18="", "",'K1'!A18)</f>
-        <v/>
-      </c>
-      <c r="B18" s="36" t="str">
+        <v>Nyhagen, Håkon</v>
+      </c>
+      <c r="B18" s="36">
         <f>IF('K1'!A18="", "",'K1'!H18)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C18" s="37" t="str">
         <f>IF('K1'!A18="", "",'K1'!I18)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D18" s="11"/>
       <c r="E18" s="25"/>
@@ -53821,15 +53841,15 @@
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="39" t="str">
         <f>IF('K1'!A19="", "",'K1'!A19)</f>
-        <v/>
-      </c>
-      <c r="B19" s="36" t="str">
+        <v>Stensvold, Trym</v>
+      </c>
+      <c r="B19" s="36">
         <f>IF('K1'!A19="", "",'K1'!H19)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C19" s="37" t="str">
         <f>IF('K1'!A19="", "",'K1'!I19)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D19" s="11"/>
       <c r="E19" s="25"/>
@@ -55920,7 +55940,7 @@
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="39" t="str">
         <f>IF('K2'!A4="", "",'K2'!A4)</f>
-        <v>Kristoffer Seegaard</v>
+        <v>Bossum, Andreas</v>
       </c>
       <c r="B4" s="36">
         <f>IF('K2'!A4="", "",'K2'!B4)</f>
@@ -55944,7 +55964,7 @@
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="39" t="str">
         <f>IF('K2'!A5="", "",'K2'!A5)</f>
-        <v>Vidar Brenna</v>
+        <v>Brenna, Vidar</v>
       </c>
       <c r="B5" s="36">
         <f>IF('K2'!A5="", "",'K2'!B5)</f>
@@ -55968,7 +55988,7 @@
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="39" t="str">
         <f>IF('K2'!A6="", "",'K2'!A6)</f>
-        <v>Marius Viken Vesterås</v>
+        <v>Flugstad, Fredrik Fuglerud</v>
       </c>
       <c r="B6" s="36">
         <f>IF('K2'!A6="", "",'K2'!B6)</f>
@@ -55992,7 +56012,7 @@
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="39" t="str">
         <f>IF('K2'!A7="", "",'K2'!A7)</f>
-        <v>Thomas Stangjordet</v>
+        <v>Moseby, Håvard</v>
       </c>
       <c r="B7" s="36">
         <f>IF('K2'!A7="", "",'K2'!B7)</f>
@@ -56016,7 +56036,7 @@
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="39" t="str">
         <f>IF('K2'!A8="", "",'K2'!A8)</f>
-        <v>Håvard Moseby</v>
+        <v>Seegaard, Kristoffer</v>
       </c>
       <c r="B8" s="36">
         <f>IF('K2'!A8="", "",'K2'!B8)</f>
@@ -56040,7 +56060,7 @@
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="39" t="str">
         <f>IF('K2'!A9="", "",'K2'!A9)</f>
-        <v>Fredrik Fuglerud Flugstad</v>
+        <v>Stangjordet, Thomas</v>
       </c>
       <c r="B9" s="36">
         <f>IF('K2'!A9="", "",'K2'!B9)</f>
@@ -56064,7 +56084,7 @@
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="39" t="str">
         <f>IF('K2'!A10="", "",'K2'!A10)</f>
-        <v>Andreas Bossum</v>
+        <v>Vesterås, Marius Viken</v>
       </c>
       <c r="B10" s="36">
         <f>IF('K2'!A10="", "",'K2'!B10)</f>
@@ -58379,7 +58399,7 @@
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="str">
         <f>IF('K2'!A4="", "",'K2'!A4)</f>
-        <v>Kristoffer Seegaard</v>
+        <v>Bossum, Andreas</v>
       </c>
       <c r="B4" s="25">
         <f>IF('K2'!A4="", "",'K2'!E4)</f>
@@ -58403,7 +58423,7 @@
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="str">
         <f>IF('K2'!A5="", "",'K2'!A5)</f>
-        <v>Vidar Brenna</v>
+        <v>Brenna, Vidar</v>
       </c>
       <c r="B5" s="25">
         <f>IF('K2'!A5="", "",'K2'!E5)</f>
@@ -58427,7 +58447,7 @@
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="str">
         <f>IF('K2'!A6="", "",'K2'!A6)</f>
-        <v>Marius Viken Vesterås</v>
+        <v>Flugstad, Fredrik Fuglerud</v>
       </c>
       <c r="B6" s="25">
         <f>IF('K2'!A6="", "",'K2'!E6)</f>
@@ -58451,7 +58471,7 @@
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="str">
         <f>IF('K2'!A7="", "",'K2'!A7)</f>
-        <v>Thomas Stangjordet</v>
+        <v>Moseby, Håvard</v>
       </c>
       <c r="B7" s="25">
         <f>IF('K2'!A7="", "",'K2'!E7)</f>
@@ -58475,7 +58495,7 @@
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="str">
         <f>IF('K2'!A8="", "",'K2'!A8)</f>
-        <v>Håvard Moseby</v>
+        <v>Seegaard, Kristoffer</v>
       </c>
       <c r="B8" s="25">
         <f>IF('K2'!A8="", "",'K2'!E8)</f>
@@ -58499,7 +58519,7 @@
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="str">
         <f>IF('K2'!A9="", "",'K2'!A9)</f>
-        <v>Fredrik Fuglerud Flugstad</v>
+        <v>Stangjordet, Thomas</v>
       </c>
       <c r="B9" s="25">
         <f>IF('K2'!A9="", "",'K2'!E9)</f>
@@ -58523,7 +58543,7 @@
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="str">
         <f>IF('K2'!A10="", "",'K2'!A10)</f>
-        <v>Andreas Bossum</v>
+        <v>Vesterås, Marius Viken</v>
       </c>
       <c r="B10" s="25">
         <f>IF('K2'!A10="", "",'K2'!E10)</f>
@@ -60840,7 +60860,7 @@
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="39" t="str">
         <f>IF('K2'!A4="", "",'K2'!A4)</f>
-        <v>Kristoffer Seegaard</v>
+        <v>Bossum, Andreas</v>
       </c>
       <c r="B4" s="36">
         <f>IF('K2'!A4="", "",'K2'!H4)</f>
@@ -60864,7 +60884,7 @@
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="39" t="str">
         <f>IF('K2'!A5="", "",'K2'!A5)</f>
-        <v>Vidar Brenna</v>
+        <v>Brenna, Vidar</v>
       </c>
       <c r="B5" s="36">
         <f>IF('K2'!A5="", "",'K2'!H5)</f>
@@ -60888,7 +60908,7 @@
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="39" t="str">
         <f>IF('K2'!A6="", "",'K2'!A6)</f>
-        <v>Marius Viken Vesterås</v>
+        <v>Flugstad, Fredrik Fuglerud</v>
       </c>
       <c r="B6" s="36">
         <f>IF('K2'!A6="", "",'K2'!H6)</f>
@@ -60912,7 +60932,7 @@
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="39" t="str">
         <f>IF('K2'!A7="", "",'K2'!A7)</f>
-        <v>Thomas Stangjordet</v>
+        <v>Moseby, Håvard</v>
       </c>
       <c r="B7" s="36">
         <f>IF('K2'!A7="", "",'K2'!H7)</f>
@@ -60936,7 +60956,7 @@
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="39" t="str">
         <f>IF('K2'!A8="", "",'K2'!A8)</f>
-        <v>Håvard Moseby</v>
+        <v>Seegaard, Kristoffer</v>
       </c>
       <c r="B8" s="36">
         <f>IF('K2'!A8="", "",'K2'!H8)</f>
@@ -60960,7 +60980,7 @@
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="39" t="str">
         <f>IF('K2'!A9="", "",'K2'!A9)</f>
-        <v>Fredrik Fuglerud Flugstad</v>
+        <v>Stangjordet, Thomas</v>
       </c>
       <c r="B9" s="36">
         <f>IF('K2'!A9="", "",'K2'!H9)</f>
@@ -60984,7 +61004,7 @@
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="39" t="str">
         <f>IF('K2'!A10="", "",'K2'!A10)</f>
-        <v>Andreas Bossum</v>
+        <v>Vesterås, Marius Viken</v>
       </c>
       <c r="B10" s="36">
         <f>IF('K2'!A10="", "",'K2'!H10)</f>

</xml_diff>